<commit_message>
added solution to baseballGame using a stack to keep track of the scores in the baseball game
</commit_message>
<xml_diff>
--- a/Algorithms/Table of Contents (Leetcode Solutions).xlsx
+++ b/Algorithms/Table of Contents (Leetcode Solutions).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesse/Desktop/interview_prep/LeetCodeSolutions-/PythonVersion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesse/Desktop/interview_prep/LeetCodeSolutions-/Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7A9FBF3-1252-CA4B-8CBC-13C88C6ED948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAD4CAC-0BF3-5D43-8A80-B210E5EEA959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7240" yWindow="780" windowWidth="18580" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">Number </t>
   </si>
@@ -69,7 +69,13 @@
     <t>Valid Pallindrome II</t>
   </si>
   <si>
-    <t>Strins</t>
+    <t xml:space="preserve">BaseballGame </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stack </t>
+  </si>
+  <si>
+    <t>Python</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -176,9 +182,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -539,7 +542,7 @@
   <dimension ref="B1:F11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -613,26 +616,37 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="4"/>
+      <c r="B7" s="4">
+        <v>682</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="5"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="5"/>
+      <c r="B11" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
added solution to contains duplicate using a set, and updated list of questions
</commit_message>
<xml_diff>
--- a/Algorithms/Table of Contents (Leetcode Solutions).xlsx
+++ b/Algorithms/Table of Contents (Leetcode Solutions).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesse/Desktop/interview_prep/LeetCodeSolutions-/Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAD4CAC-0BF3-5D43-8A80-B210E5EEA959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D851CE5-227A-AE4B-954B-398268EB1B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7240" yWindow="780" windowWidth="18580" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">Number </t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ContainsDuplicate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python </t>
   </si>
 </sst>
 </file>
@@ -542,7 +551,7 @@
   <dimension ref="B1:F11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -637,7 +646,18 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="4"/>
+      <c r="B8" s="4">
+        <v>217</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4"/>

</xml_diff>

<commit_message>
added solutions to a handful of easy questions and added them to the table of contenents as well. Next up more questions :)
</commit_message>
<xml_diff>
--- a/Algorithms/Table of Contents (Leetcode Solutions).xlsx
+++ b/Algorithms/Table of Contents (Leetcode Solutions).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesse/Desktop/interview_prep/LeetCodeSolutions-/Algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D851CE5-227A-AE4B-954B-398268EB1B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E570F897-3705-CB4D-8534-0C2DD32F8A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="780" windowWidth="18580" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17620" yWindow="760" windowWidth="15820" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
   <si>
     <t xml:space="preserve">Number </t>
   </si>
@@ -69,22 +69,199 @@
     <t>Valid Pallindrome II</t>
   </si>
   <si>
-    <t xml:space="preserve">BaseballGame </t>
-  </si>
-  <si>
     <t xml:space="preserve">Stack </t>
   </si>
   <si>
     <t>Python</t>
   </si>
   <si>
-    <t xml:space="preserve">ContainsDuplicate </t>
-  </si>
-  <si>
     <t xml:space="preserve">Set </t>
   </si>
   <si>
     <t xml:space="preserve">Python </t>
+  </si>
+  <si>
+    <t>Trees(DFS)</t>
+  </si>
+  <si>
+    <t>LinkedList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iterated thru the array and checked if the flowerpot is empyt and the next two cells are also empty then we can plant. </t>
+  </si>
+  <si>
+    <t>Used dfs technique to traverse the tree and get the in order traversal of the tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used a stack to keep track of the next greater element to the right of each value in the array. We can do this by popping the values if they smaller than the current element and for every element left in the stack there is no greater element so we set thier valeus to -1. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We iterate over the haystack and if we have the first occurrence of the needle and the string length is at least len(needle) then we check the substring to see if they match if they do we return true. </t>
+  </si>
+  <si>
+    <t>StandarQuestions (Boyer-Moore Voting alg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can solve this question by using the Boyer-Moore Voting algorithm in which we set an element to the majority element and each time we encounter a number that is not the current element we decrease the frequency of the majoriry element by one. On the other hand each time we encounter another element that is the current majority element we incresase our frequency by one. If we reach a point where the mojoirty element is less than or equal to 0 we update our majoority element. #genious solution. </t>
+  </si>
+  <si>
+    <t>DynamicProgramming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can solve this question by using dynaimc programming to remember the number of stairs at each point. </t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used a heap to keep track of the kth largest element in a stream. Each time we add a new element we make sure to pop any elements that are at the top of the heap since we are using a min heap to track at most n elemenets. </t>
+  </si>
+  <si>
+    <t>BinarySearch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We use the binary seach technique to locate an elemenet in a stream of numbers. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement stack using queues </t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For this problem we want to use a queue to work like a stack they tell us in the question we can use two separate queues but we don’t really need to we can just use one queue and for the pop operation that will be O(n) time since we will need to pop every element and then leave the last one out and push everything else back into the queue. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sqaures of  a sorted Array </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Pointers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can use the two pointer technique since the array is alreadu sorted so we can just add each item from either the left or right after we square it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word Pattern </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HashTable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseball Game </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains Duplicate </t>
+  </si>
+  <si>
+    <t>Contstruct String From Binary Search String</t>
+  </si>
+  <si>
+    <t>Remove Duplictes From Sorted Linked List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse String </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can Place Flowers </t>
+  </si>
+  <si>
+    <t>Binary Inorder Traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next Greater Element </t>
+  </si>
+  <si>
+    <t>find The Index Of The First Occurrence In A String</t>
+  </si>
+  <si>
+    <t>Majority Element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min Cost Climbning Stairs </t>
+  </si>
+  <si>
+    <t>Kth Largest Element In A Stream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary Search </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used a hasatable and a set to make sure we can uniquely map every word in our string with a letter in our pattern. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path Sum </t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can traverse the tree using a tree travesal algorithm in this case dfs and for each node we will add the current value to the path. When we reach a leaf node (i.e has no children) we can can check the sum of the path and if we have targetsum we return true </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid Perfect Sqaure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To find out if the input number is a valid perfect square we can sqare each number from 1 to N and see if any values match but we can do this even better by using binary search since we a have a sorted rage of numbers if we find a valid sum we return true else false. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move Zeros </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can iterate over our input array and whenever we find a value that is not zeros we will move it to the leftmost position we do this by using two pointers and once the rightmost pointer reaches the end we exit. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Pivot Index </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can solve this question by first adding all the values in the array and then we iterate over each element and for each element we will subtract it from the total and compare our currentSum with the totalSum and if we have a match we return the index. If we reach the end of the arrray then we have no pivot index so we return -1. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find all numbers dissappapered in an array </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclic Sort </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can solve this question by using the fact that we are going to have only numbers in a given range that is the same length of the array so we can use the "cyclic sort" teqnique in which we place all the values into their repective slots and then just iterate over the array again to find the missing values </t>
+  </si>
+  <si>
+    <t>Maximum Number of ballons</t>
+  </si>
+  <si>
+    <t>We can solve thisby using a hashtable to count the number of occureneces of each character and include only the once in the word ballon. We then just find the min number of occorrences in that set (for l and o we divdide by 2 since we need 2 of each)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guess Number Higher or Lower </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are told we are given a range of numbers from 1 to N so we should automatically think about binary search as a potential solution which in this case works and we use it to solve the guessing game. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single Number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are told that every number appears at least twice except for one of them and we want to find that number we can use xor to solve this. Since xor will give you 0 if you xor a number with itself in this case all the duplicate numbers and xor will give you the number back if it is xor with 0 so in this case we can have 0^n and get n back </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intersection of Two Linked List </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can solve this by iterating over both list one at a time if we reach the end of one list we set its pointer to the front of the opposite list until we have both list reaching the same node which can either be the intersection node or the nullpointer in which case we return null </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rearrangin Coins </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To solve this question we will iterate over a range of numbers and for each iteratation if we can complete the current step we increment our step completion count. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SlidingWindow </t>
   </si>
 </sst>
 </file>
@@ -177,7 +354,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -191,6 +368,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -260,8 +440,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="List" displayName="List" ref="B3:F11" totalsRowShown="0">
-  <autoFilter ref="B3:F11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="List" displayName="List" ref="B3:F41" totalsRowShown="0">
+  <autoFilter ref="B3:F41" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:F11">
     <sortCondition ref="B3:B11"/>
   </sortState>
@@ -548,20 +728,21 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:F11"/>
+  <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="7" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="255.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -636,13 +817,13 @@
         <v>682</v>
       </c>
       <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
@@ -650,23 +831,440 @@
         <v>217</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="4">
+        <v>606</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="4">
+        <v>83</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="4"/>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="4"/>
+      <c r="B11" s="4">
+        <v>344</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="5">
+        <v>605</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="5">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="5">
+        <v>496</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="5">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="5">
+        <v>169</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="5">
+        <v>746</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="5">
+        <v>703</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="5">
+        <v>704</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="5">
+        <v>225</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="5">
+        <v>977</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="5">
+        <v>290</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="5">
+        <v>112</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="5">
+        <v>367</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="5">
+        <v>283</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="5">
+        <v>724</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="5">
+        <v>448</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="5">
+        <v>1189</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="5">
+        <v>374</v>
+      </c>
+      <c r="C29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="5">
+        <v>136</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="5">
+        <v>160</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="5">
+        <v>441</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="5"/>
+    </row>
+    <row r="37" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>